<commit_message>
feat(profile): implement profile management commands
  - Add get-profile command with multiple ID lookup options (user-id, email,
  usbc_id, tnba_id)
  - Add edit-profile command for updating profile fields (first, last, phone,
  address)
  - Add delete-profile command with confirmation requirement
  - Add Rich table formatting for profile display with minimal borders
  - Add comprehensive test suite with 25 test cases
  - Update CLI reference documentation with multi-line command examples
  - Fix field name consistency (usbc_id/tnba_id use underscores)
  - Add rich dependency to requirements.txt
  - All commands follow ERROR: prefix standard and proper exit codes
  - Achieve 95% test coverage (exceeds 85% requirement)

  🤖 Generated with [Claude Code](https://claude.ai/code)

  Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/pre-planning/4thArrowFunctions.xlsx
+++ b/docs/pre-planning/4thArrowFunctions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewwtennant/Documents/Code/4th_Arrow_Tournament_Control/docs/pre-planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57EBD009-820C-A046-9B39-0071A06FD400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F5AF57-9891-0944-A992-0351DBD19A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35620" yWindow="2780" windowWidth="27640" windowHeight="16940" xr2:uid="{F23FF352-42BB-3F43-90C1-546E421826C7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
   <si>
     <t>Function</t>
   </si>
@@ -144,13 +144,136 @@
   </si>
   <si>
     <t>Create Non-members (bowlers)</t>
+  </si>
+  <si>
+    <t>Create Fliers</t>
+  </si>
+  <si>
+    <t>Create Rules</t>
+  </si>
+  <si>
+    <t>Tournament Control (Day of)</t>
+  </si>
+  <si>
+    <t>Add Bowlers</t>
+  </si>
+  <si>
+    <t>Add Workers</t>
+  </si>
+  <si>
+    <t>Set Worker Roles</t>
+  </si>
+  <si>
+    <t>Task Management</t>
+  </si>
+  <si>
+    <t>Determine Todo dates</t>
+  </si>
+  <si>
+    <t>To Dos</t>
+  </si>
+  <si>
+    <t>Finish Own Profile</t>
+  </si>
+  <si>
+    <t>Merge Member Profiles</t>
+  </si>
+  <si>
+    <t>Sanction Tournaments (if app)</t>
+  </si>
+  <si>
+    <t>Create Fliers (if app)</t>
+  </si>
+  <si>
+    <t>Center Financial Agreement</t>
+  </si>
+  <si>
+    <t>Edit Entries</t>
+  </si>
+  <si>
+    <t>Enter Bowlers in Side Action</t>
+  </si>
+  <si>
+    <t>Enter Scores</t>
+  </si>
+  <si>
+    <t>Collect Scores by Camera</t>
+  </si>
+  <si>
+    <t>Collect Scores Remotely</t>
+  </si>
+  <si>
+    <t>Create Brackets</t>
+  </si>
+  <si>
+    <t>Go to next Game</t>
+  </si>
+  <si>
+    <t>Set 'Smart Button Rules</t>
+  </si>
+  <si>
+    <t>'Smart Button'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t>Create Prize List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tournament Income/Outgo </t>
+  </si>
+  <si>
+    <t>Pre-payments</t>
+  </si>
+  <si>
+    <t>Day-of payments</t>
+  </si>
+  <si>
+    <t>Brackets</t>
+  </si>
+  <si>
+    <t>Jackpots</t>
+  </si>
+  <si>
+    <t>Eliminators</t>
+  </si>
+  <si>
+    <t>Big Boards</t>
+  </si>
+  <si>
+    <t>Create Side Action Sheets</t>
+  </si>
+  <si>
+    <t>Create Financial Reports- tournament</t>
+  </si>
+  <si>
+    <t>Create Financial Reports- organization</t>
+  </si>
+  <si>
+    <t>Contact Bowlers</t>
+  </si>
+  <si>
+    <t>Sort Standings</t>
+  </si>
+  <si>
+    <t>Update Side Action</t>
+  </si>
+  <si>
+    <t>Determine final financial structure</t>
+  </si>
+  <si>
+    <t>Side Action Finance Management- day of</t>
+  </si>
+  <si>
+    <t>Create Todos from other systems</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -179,8 +302,22 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="0.79998168889431442"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,8 +336,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -208,17 +357,121 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,261 +806,1190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F972E6-8630-6F4B-881D-13BC7C61B359}">
-  <dimension ref="A2:H37"/>
+  <dimension ref="A1:V63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="2" max="8" width="32.33203125" customWidth="1"/>
+    <col min="2" max="6" width="32.33203125" customWidth="1"/>
+    <col min="7" max="7" width="34.1640625" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:22" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E3" s="10"/>
+      <c r="F3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="12"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="14"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="14"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="14"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="14"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="14"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="14"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="14"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="14"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="14"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="14"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="14"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="14"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="14"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="14"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="14"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="14"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="14"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F21" s="7"/>
+      <c r="G21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="14"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F22" s="7"/>
+      <c r="G22" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="14"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="G23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="14"/>
+    </row>
+    <row r="24" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="16"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C25" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D25" s="7"/>
+      <c r="E25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="14"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="14"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="14"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="14"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="14"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="14"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="14"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="14"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="14"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="14"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13"/>
+      <c r="S35" s="13"/>
+      <c r="T35" s="13"/>
+      <c r="U35" s="13"/>
+      <c r="V35" s="14"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="14"/>
+    </row>
+    <row r="37" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="R37" s="17"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="17"/>
+      <c r="U37" s="17"/>
+      <c r="V37" s="18"/>
+    </row>
+    <row r="38" spans="1:22" s="19" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="19" t="str">
+        <f>B2</f>
+        <v>User Management</v>
+      </c>
+      <c r="C38" s="19" t="str">
+        <f t="shared" ref="C38:M38" si="0">C2</f>
+        <v>Organization Management</v>
+      </c>
+      <c r="D38" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Tournament Management</v>
+      </c>
+      <c r="E38" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Marketing Management</v>
+      </c>
+      <c r="F38" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Tournament Control (Day of)</v>
+      </c>
+      <c r="G38" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Financial Management</v>
+      </c>
+      <c r="H38" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Side Action Management</v>
+      </c>
+      <c r="I38" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Task Management</v>
+      </c>
+      <c r="J38" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K38" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L38" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M38" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A39" s="20"/>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" t="s">
+        <v>47</v>
+      </c>
+      <c r="F39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A40" s="21"/>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A41" s="21"/>
+      <c r="D41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A42" s="21"/>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A43" s="21"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A44" s="21"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A45" s="21"/>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A46" s="21"/>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A47" s="21"/>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A48" s="21"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="21"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="21"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="21"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="21"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="21"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="21"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="21"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="21"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="21"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="21"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="21"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="21"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="21"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="21"/>
+    </row>
+    <row r="63" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>